<commit_message>
SPRINT C - ATRIBUIÇÃO DE USs
</commit_message>
<xml_diff>
--- a/docs/Planeamento/SPRINT C/US_SprintC - PLANEAMENTO.xlsx
+++ b/docs/Planeamento/SPRINT C/US_SprintC - PLANEAMENTO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luism\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luism\Desktop\lei20_21_s4_2dl_4\docs\Planeamento\SPRINT C\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8C550FD-32D7-4FBF-96EA-FEAB5529E802}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A12D80-A388-4884-9EDF-EFCC48579DB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FDCDD7A7-A42D-BB49-A3F1-83703FDDB978}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="71">
   <si>
     <t>UC</t>
   </si>
@@ -254,6 +254,39 @@
   </si>
   <si>
     <t>SIM</t>
+  </si>
+  <si>
+    <t>ASSIGNADO</t>
+  </si>
+  <si>
+    <t>LUIS</t>
+  </si>
+  <si>
+    <t>SERGIO/TIAGO</t>
+  </si>
+  <si>
+    <t>FAUSTO/JOAO</t>
+  </si>
+  <si>
+    <t>FAUSTO</t>
+  </si>
+  <si>
+    <t>TIAGO/JOAO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERGIO </t>
+  </si>
+  <si>
+    <t>JOAO</t>
+  </si>
+  <si>
+    <t>FAUSTO/TIAGO</t>
+  </si>
+  <si>
+    <t>LUIS/JOAO</t>
+  </si>
+  <si>
+    <t>SERGIO</t>
   </si>
 </sst>
 </file>
@@ -298,7 +331,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +353,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -360,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -407,6 +446,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -740,11 +785,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5B1A8D-0180-0642-B118-F58C3A59AAC7}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -757,10 +802,11 @@
     <col min="7" max="7" width="75.796875" style="2" customWidth="1"/>
     <col min="8" max="8" width="19.296875" style="1" customWidth="1"/>
     <col min="9" max="9" width="79.5" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="10.796875" style="3"/>
+    <col min="10" max="10" width="15.3984375" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="10.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>58</v>
       </c>
@@ -788,8 +834,11 @@
       <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="78" x14ac:dyDescent="0.3">
+      <c r="J1" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="78" x14ac:dyDescent="0.3">
       <c r="B2" s="12">
         <v>5</v>
       </c>
@@ -814,8 +863,11 @@
       <c r="I2" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="88.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="88.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
@@ -840,8 +892,11 @@
       <c r="H3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="J3" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
@@ -866,8 +921,11 @@
       <c r="H4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="82.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J4" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="82.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -892,8 +950,11 @@
       <c r="I5" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="J5" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -915,8 +976,11 @@
       <c r="H6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="J6" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -941,8 +1005,11 @@
       <c r="I7" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" s="11" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J7" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="11" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>5</v>
       </c>
@@ -967,8 +1034,11 @@
       <c r="I8" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="J8" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>2</v>
       </c>
@@ -990,8 +1060,11 @@
       <c r="H9" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>59</v>
       </c>
@@ -1019,8 +1092,11 @@
       <c r="I10" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="J10" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>59</v>
       </c>
@@ -1048,8 +1124,11 @@
       <c r="I11" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J11" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="87" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>8</v>
       </c>
@@ -1074,8 +1153,11 @@
       <c r="I12" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="J12" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>1</v>
       </c>
@@ -1100,8 +1182,11 @@
       <c r="I13" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="78" x14ac:dyDescent="0.3">
+      <c r="J13" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="78" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>8</v>
       </c>
@@ -1126,8 +1211,11 @@
       <c r="I14" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="J14" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>5</v>
       </c>
@@ -1152,8 +1240,11 @@
       <c r="I15" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J15" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>1</v>
       </c>
@@ -1178,6 +1269,12 @@
       <c r="I16" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="J16" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J17" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:I16" xr:uid="{BF8C8512-301D-2D43-8EDD-4BC55BF43399}">

</xml_diff>

<commit_message>
SPRINT C - PLANEAMENTO
</commit_message>
<xml_diff>
--- a/docs/Planeamento/SPRINT C/US_SprintC - PLANEAMENTO.xlsx
+++ b/docs/Planeamento/SPRINT C/US_SprintC - PLANEAMENTO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luism\Desktop\lei20_21_s4_2dl_4\docs\Planeamento\SPRINT C\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A12D80-A388-4884-9EDF-EFCC48579DB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B00F49-76AC-436A-829B-F77A456977F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FDCDD7A7-A42D-BB49-A3F1-83703FDDB978}"/>
   </bookViews>
@@ -262,9 +262,6 @@
     <t>LUIS</t>
   </si>
   <si>
-    <t>SERGIO/TIAGO</t>
-  </si>
-  <si>
     <t>FAUSTO/JOAO</t>
   </si>
   <si>
@@ -287,6 +284,9 @@
   </si>
   <si>
     <t>SERGIO</t>
+  </si>
+  <si>
+    <t>TIAGO</t>
   </si>
 </sst>
 </file>
@@ -789,7 +789,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -893,7 +893,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
@@ -921,8 +921,8 @@
       <c r="H4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>63</v>
+      <c r="J4" s="18" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="82.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -951,7 +951,7 @@
         <v>51</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
@@ -1006,7 +1006,7 @@
         <v>52</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="11" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
@@ -1035,7 +1035,7 @@
         <v>12</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
@@ -1061,7 +1061,7 @@
         <v>4</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.3">
@@ -1093,7 +1093,7 @@
         <v>53</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="93.6" x14ac:dyDescent="0.3">
@@ -1125,7 +1125,7 @@
         <v>54</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="87" customHeight="1" x14ac:dyDescent="0.3">
@@ -1154,7 +1154,7 @@
         <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -1183,7 +1183,7 @@
         <v>19</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="78" x14ac:dyDescent="0.3">
@@ -1241,7 +1241,7 @@
         <v>22</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1270,7 +1270,7 @@
         <v>18</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="10:10" x14ac:dyDescent="0.3">
@@ -1293,7 +1293,8 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>

<commit_message>
<LDG-29> Daily meeting e assignação de USs
</commit_message>
<xml_diff>
--- a/docs/Planeamento/SPRINT C/US_SprintC - PLANEAMENTO.xlsx
+++ b/docs/Planeamento/SPRINT C/US_SprintC - PLANEAMENTO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luism\Desktop\lei20_21_s4_2dl_4\docs\Planeamento\SPRINT C\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B00F49-76AC-436A-829B-F77A456977F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACBDC5F-0374-4E89-AF03-43568969B791}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FDCDD7A7-A42D-BB49-A3F1-83703FDDB978}"/>
   </bookViews>
@@ -788,8 +788,8 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1173,7 +1173,7 @@
       <c r="F13" s="1">
         <v>2104</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="16" t="s">
         <v>20</v>
       </c>
       <c r="H13" s="1" t="s">

</xml_diff>

<commit_message>
<LDG-34> Classe Ticket e FormularioPreenchido adicionadas
</commit_message>
<xml_diff>
--- a/docs/Planeamento/SPRINT C/US_SprintC - PLANEAMENTO.xlsx
+++ b/docs/Planeamento/SPRINT C/US_SprintC - PLANEAMENTO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luism\Desktop\lei20_21_s4_2dl_4\docs\Planeamento\SPRINT C\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACBDC5F-0374-4E89-AF03-43568969B791}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CF1CAA-E689-4F6E-A454-5512BA7CA42C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FDCDD7A7-A42D-BB49-A3F1-83703FDDB978}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="72">
   <si>
     <t>UC</t>
   </si>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t>TIAGO</t>
+  </si>
+  <si>
+    <t>LUIS/FAUSTO</t>
   </si>
 </sst>
 </file>
@@ -788,15 +791,16 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.796875" style="3"/>
-    <col min="2" max="3" width="10.796875" style="1"/>
-    <col min="4" max="4" width="18.796875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="15.8984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" style="1"/>
+    <col min="4" max="4" width="21.5" style="8" customWidth="1"/>
     <col min="5" max="5" width="8.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.796875" style="1"/>
     <col min="7" max="7" width="75.796875" style="2" customWidth="1"/>
@@ -839,6 +843,9 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="78" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B2" s="12">
         <v>5</v>
       </c>
@@ -864,7 +871,7 @@
         <v>17</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="88.05" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
<LDG-28> Resolução bug na UI
</commit_message>
<xml_diff>
--- a/docs/Planeamento/SPRINT C/US_SprintC - PLANEAMENTO.xlsx
+++ b/docs/Planeamento/SPRINT C/US_SprintC - PLANEAMENTO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luism\Desktop\lei20_21_s4_2dl_4\docs\Planeamento\SPRINT C\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CF1CAA-E689-4F6E-A454-5512BA7CA42C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FB488B-6EE7-4CCC-9C49-4DE23C4DF4A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FDCDD7A7-A42D-BB49-A3F1-83703FDDB978}"/>
   </bookViews>
@@ -792,7 +792,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>